<commit_message>
Changues for the lastest version
</commit_message>
<xml_diff>
--- a/data/mas_original_results.xlsx
+++ b/data/mas_original_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univmurcia-my.sharepoint.com/personal/ruben_lopez15_um_es/Documents/FPU2018/Tesis/Drafts/Paper 2/Project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univmurcia-my.sharepoint.com/personal/rlopez_um_es/Documents/FPU2018/meta-analyses_reproducibility_bueno/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1164" documentId="8_{CDF712D2-BC8B-4E3C-8B27-05363CDCB4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FC6896B-507E-40C4-B9DC-D7F66A7A52E4}"/>
+  <xr:revisionPtr revIDLastSave="1166" documentId="8_{CDF712D2-BC8B-4E3C-8B27-05363CDCB4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{448B4664-CCC8-4C9F-B6FC-E138079F13BB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3469" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3471" uniqueCount="818">
   <si>
     <t>order</t>
   </si>
@@ -2633,7 +2633,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -3015,11 +3015,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="W49" sqref="W49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
@@ -3153,6 +3153,9 @@
       <c r="G2" t="s">
         <v>36</v>
       </c>
+      <c r="J2" t="s">
+        <v>51</v>
+      </c>
       <c r="K2" t="s">
         <v>37</v>
       </c>
@@ -3220,6 +3223,9 @@
       </c>
       <c r="G3" t="s">
         <v>43</v>
+      </c>
+      <c r="J3" t="s">
+        <v>51</v>
       </c>
       <c r="K3" t="s">
         <v>37</v>
@@ -19802,7 +19808,7 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
   </cols>

</xml_diff>